<commit_message>
atualizei as colunas da planilha de notas de ES
</commit_message>
<xml_diff>
--- a/aulas/gsi526/notas_esof_cefet_2019.xlsx
+++ b/aulas/gsi526/notas_esof_cefet_2019.xlsx
@@ -31,21 +31,12 @@
     <t>P2 (25)</t>
   </si>
   <si>
-    <t>L2 (2,5)</t>
-  </si>
-  <si>
     <t>P3 (30)</t>
   </si>
   <si>
-    <t>L3 (2,5)</t>
-  </si>
-  <si>
     <t>S (15)</t>
   </si>
   <si>
-    <t>Situação</t>
-  </si>
-  <si>
     <t>A = Aprovado</t>
   </si>
   <si>
@@ -74,6 +65,15 @@
   </si>
   <si>
     <t>Excel 97-2003</t>
+  </si>
+  <si>
+    <t>L (2,5)</t>
+  </si>
+  <si>
+    <t>L(2,5)</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -107,21 +107,23 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF00B050"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Verdana"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -209,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -227,9 +229,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -241,7 +241,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -253,6 +253,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,15 +623,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.44140625" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" customWidth="1"/>
-    <col min="8" max="8" width="12.77734375" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" customWidth="1"/>
+    <col min="3" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" customWidth="1"/>
+    <col min="6" max="6" width="8.77734375" customWidth="1"/>
+    <col min="7" max="7" width="9.44140625" customWidth="1"/>
+    <col min="8" max="8" width="8.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
@@ -642,19 +649,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>6</v>
-      </c>
       <c r="H1" s="5" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
@@ -1179,15 +1186,17 @@
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H32" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H33" s="7" t="s">
-        <v>9</v>
-      </c>
+    <row r="32" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="G32" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="H32" s="16"/>
+    </row>
+    <row r="33" spans="7:8" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="G33" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H33" s="16"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -1216,92 +1225,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+    </row>
+    <row r="4" spans="2:6" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="B4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+    </row>
+    <row r="6" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-    </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+      <c r="C6" s="7"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-    </row>
-    <row r="4" spans="2:6" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
+      <c r="F6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-    </row>
-    <row r="6" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B6" s="9" t="s">
+    </row>
+    <row r="7" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+    </row>
+    <row r="8" spans="2:6" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13" t="s">
+      <c r="C8" s="10"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13">
+        <v>1</v>
+      </c>
+      <c r="F8" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-    </row>
-    <row r="8" spans="2:6" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15">
-        <v>1</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
notas da prova 3 de ES
</commit_message>
<xml_diff>
--- a/aulas/gsi526/notas_esof_cefet_2019.xlsx
+++ b/aulas/gsi526/notas_esof_cefet_2019.xlsx
@@ -83,17 +83,11 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b/>
@@ -124,6 +118,17 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -211,25 +216,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -241,7 +243,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -253,9 +255,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -623,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -635,32 +644,32 @@
     <col min="5" max="5" width="9.109375" customWidth="1"/>
     <col min="6" max="6" width="8.77734375" customWidth="1"/>
     <col min="7" max="7" width="9.44140625" customWidth="1"/>
-    <col min="8" max="8" width="8.109375" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -674,13 +683,15 @@
       <c r="C2" s="2">
         <v>21</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="17">
+        <v>30</v>
+      </c>
       <c r="E2" s="2">
         <v>1.5</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -692,13 +703,15 @@
       <c r="C3" s="2">
         <v>25</v>
       </c>
-      <c r="D3" s="3"/>
+      <c r="D3" s="17">
+        <v>30</v>
+      </c>
       <c r="E3" s="2">
         <v>2.5</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -710,13 +723,15 @@
       <c r="C4" s="2">
         <v>17</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="17">
+        <v>25</v>
+      </c>
       <c r="E4" s="2">
         <v>2.5</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -728,13 +743,15 @@
       <c r="C5" s="2">
         <v>16</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="17">
+        <v>25</v>
+      </c>
       <c r="E5" s="2">
         <v>1.5</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -746,13 +763,15 @@
       <c r="C6" s="2">
         <v>19.5</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="17">
+        <v>25</v>
+      </c>
       <c r="E6" s="2">
         <v>1.5</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -764,13 +783,15 @@
       <c r="C7" s="2">
         <v>17</v>
       </c>
-      <c r="D7" s="3"/>
+      <c r="D7" s="17">
+        <v>25</v>
+      </c>
       <c r="E7" s="2">
         <v>2.5</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -782,13 +803,15 @@
       <c r="C8" s="2">
         <v>19.5</v>
       </c>
-      <c r="D8" s="3"/>
+      <c r="D8" s="17">
+        <v>25</v>
+      </c>
       <c r="E8" s="2">
         <v>0</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -800,13 +823,15 @@
       <c r="C9" s="2">
         <v>16</v>
       </c>
-      <c r="D9" s="3"/>
+      <c r="D9" s="17">
+        <v>30</v>
+      </c>
       <c r="E9" s="2">
         <v>1.5</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -818,13 +843,15 @@
       <c r="C10" s="2">
         <v>19.5</v>
       </c>
-      <c r="D10" s="3"/>
+      <c r="D10" s="17">
+        <v>30</v>
+      </c>
       <c r="E10" s="2">
         <v>2.5</v>
       </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -836,13 +863,15 @@
       <c r="C11" s="2">
         <v>25</v>
       </c>
-      <c r="D11" s="3"/>
+      <c r="D11" s="17">
+        <v>30</v>
+      </c>
       <c r="E11" s="2">
         <v>2.5</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -854,13 +883,15 @@
       <c r="C12" s="2">
         <v>18.5</v>
       </c>
-      <c r="D12" s="3"/>
+      <c r="D12" s="17">
+        <v>20</v>
+      </c>
       <c r="E12" s="2">
         <v>0</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -872,13 +903,15 @@
       <c r="C13" s="2">
         <v>21</v>
       </c>
-      <c r="D13" s="3"/>
+      <c r="D13" s="17">
+        <v>30</v>
+      </c>
       <c r="E13" s="2">
         <v>2.5</v>
       </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -890,13 +923,15 @@
       <c r="C14" s="2">
         <v>22.5</v>
       </c>
-      <c r="D14" s="3"/>
+      <c r="D14" s="17">
+        <v>25</v>
+      </c>
       <c r="E14" s="2">
         <v>1</v>
       </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="3"/>
     </row>
     <row r="15" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -908,13 +943,15 @@
       <c r="C15" s="2">
         <v>25</v>
       </c>
-      <c r="D15" s="3"/>
+      <c r="D15" s="17">
+        <v>25</v>
+      </c>
       <c r="E15" s="2">
         <v>2.5</v>
       </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -926,13 +963,15 @@
       <c r="C16" s="2">
         <v>20</v>
       </c>
-      <c r="D16" s="4"/>
+      <c r="D16" s="18">
+        <v>30</v>
+      </c>
       <c r="E16" s="2">
         <v>1</v>
       </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
@@ -944,13 +983,15 @@
       <c r="C17" s="2">
         <v>15.5</v>
       </c>
-      <c r="D17" s="4"/>
+      <c r="D17" s="18">
+        <v>30</v>
+      </c>
       <c r="E17" s="2">
         <v>1</v>
       </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
@@ -962,13 +1003,15 @@
       <c r="C18" s="2">
         <v>17</v>
       </c>
-      <c r="D18" s="4"/>
+      <c r="D18" s="18">
+        <v>30</v>
+      </c>
       <c r="E18" s="2">
         <v>2.5</v>
       </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="3"/>
     </row>
     <row r="19" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
@@ -980,13 +1023,15 @@
       <c r="C19" s="2">
         <v>21</v>
       </c>
-      <c r="D19" s="4"/>
+      <c r="D19" s="18">
+        <v>25</v>
+      </c>
       <c r="E19" s="2">
         <v>2.5</v>
       </c>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
@@ -998,13 +1043,15 @@
       <c r="C20" s="2">
         <v>19.5</v>
       </c>
-      <c r="D20" s="4"/>
+      <c r="D20" s="18">
+        <v>30</v>
+      </c>
       <c r="E20" s="2">
         <v>1.5</v>
       </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="3"/>
     </row>
     <row r="21" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
@@ -1016,13 +1063,15 @@
       <c r="C21" s="2">
         <v>13</v>
       </c>
-      <c r="D21" s="4"/>
+      <c r="D21" s="18">
+        <v>25</v>
+      </c>
       <c r="E21" s="2">
         <v>0</v>
       </c>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="3"/>
     </row>
     <row r="22" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
@@ -1034,13 +1083,15 @@
       <c r="C22" s="2">
         <v>18.5</v>
       </c>
-      <c r="D22" s="4"/>
+      <c r="D22" s="18">
+        <v>30</v>
+      </c>
       <c r="E22" s="2">
         <v>1</v>
       </c>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="3"/>
     </row>
     <row r="23" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
@@ -1052,13 +1103,15 @@
       <c r="C23" s="2">
         <v>25</v>
       </c>
-      <c r="D23" s="4"/>
+      <c r="D23" s="18">
+        <v>30</v>
+      </c>
       <c r="E23" s="2">
         <v>1.5</v>
       </c>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="3"/>
     </row>
     <row r="24" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
@@ -1070,13 +1123,15 @@
       <c r="C24" s="2">
         <v>25</v>
       </c>
-      <c r="D24" s="4"/>
+      <c r="D24" s="18">
+        <v>25</v>
+      </c>
       <c r="E24" s="2">
         <v>1.5</v>
       </c>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="3"/>
     </row>
     <row r="25" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
@@ -1088,13 +1143,15 @@
       <c r="C25" s="2">
         <v>17</v>
       </c>
-      <c r="D25" s="4"/>
+      <c r="D25" s="18">
+        <v>25</v>
+      </c>
       <c r="E25" s="2">
         <v>1</v>
       </c>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="3"/>
     </row>
     <row r="26" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
@@ -1106,13 +1163,15 @@
       <c r="C26" s="2">
         <v>18.5</v>
       </c>
-      <c r="D26" s="4"/>
+      <c r="D26" s="18">
+        <v>30</v>
+      </c>
       <c r="E26" s="2">
         <v>2.5</v>
       </c>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="3"/>
     </row>
     <row r="27" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
@@ -1124,13 +1183,15 @@
       <c r="C27" s="2">
         <v>21</v>
       </c>
-      <c r="D27" s="4"/>
+      <c r="D27" s="18">
+        <v>25</v>
+      </c>
       <c r="E27" s="2">
         <v>2.5</v>
       </c>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="3"/>
     </row>
     <row r="28" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
@@ -1142,13 +1203,15 @@
       <c r="C28" s="2">
         <v>25</v>
       </c>
-      <c r="D28" s="4"/>
+      <c r="D28" s="18">
+        <v>30</v>
+      </c>
       <c r="E28" s="2">
         <v>2.5</v>
       </c>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="3"/>
     </row>
     <row r="29" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
@@ -1160,13 +1223,15 @@
       <c r="C29" s="2">
         <v>21</v>
       </c>
-      <c r="D29" s="4"/>
+      <c r="D29" s="18">
+        <v>30</v>
+      </c>
       <c r="E29" s="2">
         <v>2.5</v>
       </c>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="3"/>
     </row>
     <row r="30" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
@@ -1178,25 +1243,27 @@
       <c r="C30" s="2">
         <v>22.5</v>
       </c>
-      <c r="D30" s="4"/>
+      <c r="D30" s="18">
+        <v>30</v>
+      </c>
       <c r="E30" s="2">
         <v>2.5</v>
       </c>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="3"/>
     </row>
     <row r="32" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="G32" s="15" t="s">
+      <c r="G32" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="H32" s="16"/>
+      <c r="H32" s="15"/>
     </row>
     <row r="33" spans="7:8" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="G33" s="17" t="s">
+      <c r="G33" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H33" s="16"/>
+      <c r="H33" s="15"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -1225,92 +1292,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
     </row>
     <row r="4" spans="2:6" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11" t="s">
+      <c r="C6" s="6"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
     </row>
     <row r="8" spans="2:6" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13">
+      <c r="C8" s="9"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12">
         <v>1</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="13" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
notas finais de Engenharia de Software
</commit_message>
<xml_diff>
--- a/aulas/gsi526/notas_esof_cefet_2019.xlsx
+++ b/aulas/gsi526/notas_esof_cefet_2019.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Blog\aulas\gsi526\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\root_\OneDrive\Área de Trabalho\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="20">
   <si>
     <t xml:space="preserve">Matrícula </t>
   </si>
@@ -74,6 +74,12 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -83,21 +89,10 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Verdana"/>
       <family val="2"/>
     </font>
     <font>
@@ -108,27 +103,32 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF00B050"/>
       <name val="Verdana"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
       <name val="Verdana"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Verdana"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -216,22 +216,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -243,7 +230,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -255,16 +242,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -630,640 +632,908 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" customWidth="1"/>
-    <col min="3" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" customWidth="1"/>
-    <col min="6" max="6" width="8.77734375" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" customWidth="1"/>
-    <col min="8" max="8" width="9.5546875" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" customWidth="1"/>
+    <col min="6" max="6" width="7.88671875" customWidth="1"/>
+    <col min="7" max="7" width="8" customWidth="1"/>
+    <col min="8" max="8" width="7" customWidth="1"/>
+    <col min="9" max="9" width="7.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="4" t="s">
+      <c r="F1" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
         <v>201712040146</v>
       </c>
-      <c r="B2" s="2">
-        <v>15</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B2" s="12">
+        <v>15</v>
+      </c>
+      <c r="C2" s="12">
         <v>21</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="12">
         <v>30</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="12">
         <v>1.5</v>
       </c>
-      <c r="F2" s="19"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="F2" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="G2" s="12">
+        <v>15</v>
+      </c>
+      <c r="H2" s="12">
+        <v>85</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
         <v>201712040430</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="12">
         <v>20</v>
       </c>
-      <c r="C3" s="2">
-        <v>25</v>
-      </c>
-      <c r="D3" s="17">
+      <c r="C3" s="12">
+        <v>25</v>
+      </c>
+      <c r="D3" s="12">
         <v>30</v>
       </c>
-      <c r="E3" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="E3" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="F3" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="G3" s="12">
+        <v>15</v>
+      </c>
+      <c r="H3" s="12">
+        <v>95</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
         <v>201622040406</v>
       </c>
-      <c r="B4" s="2">
-        <v>25</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="B4" s="12">
+        <v>25</v>
+      </c>
+      <c r="C4" s="12">
         <v>17</v>
       </c>
-      <c r="D4" s="17">
-        <v>25</v>
-      </c>
-      <c r="E4" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="F4" s="19"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="3"/>
-    </row>
-    <row r="5" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="D4" s="12">
+        <v>25</v>
+      </c>
+      <c r="E4" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="F4" s="12">
+        <v>0</v>
+      </c>
+      <c r="G4" s="12">
+        <v>0</v>
+      </c>
+      <c r="H4" s="12">
+        <v>70</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
         <v>201622040139</v>
       </c>
-      <c r="B5" s="2">
-        <v>15</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="B5" s="12">
+        <v>15</v>
+      </c>
+      <c r="C5" s="12">
         <v>16</v>
       </c>
-      <c r="D5" s="17">
-        <v>25</v>
-      </c>
-      <c r="E5" s="2">
+      <c r="D5" s="12">
+        <v>25</v>
+      </c>
+      <c r="E5" s="12">
         <v>1.5</v>
       </c>
-      <c r="F5" s="19"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="F5" s="12">
+        <v>0</v>
+      </c>
+      <c r="G5" s="12">
+        <v>15</v>
+      </c>
+      <c r="H5" s="12">
+        <v>73</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
         <v>201712040057</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="12">
         <v>20</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="12">
         <v>19.5</v>
       </c>
-      <c r="D6" s="17">
-        <v>25</v>
-      </c>
-      <c r="E6" s="2">
+      <c r="D6" s="12">
+        <v>25</v>
+      </c>
+      <c r="E6" s="12">
         <v>1.5</v>
       </c>
-      <c r="F6" s="19"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="3"/>
-    </row>
-    <row r="7" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="F6" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="G6" s="12">
+        <v>15</v>
+      </c>
+      <c r="H6" s="12">
+        <v>84</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
         <v>201612040284</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="12">
         <v>10</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="12">
         <v>17</v>
       </c>
-      <c r="D7" s="17">
-        <v>25</v>
-      </c>
-      <c r="E7" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="F7" s="19"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="D7" s="12">
+        <v>25</v>
+      </c>
+      <c r="E7" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="F7" s="12">
+        <v>1</v>
+      </c>
+      <c r="G7" s="12">
+        <v>15</v>
+      </c>
+      <c r="H7" s="12">
+        <v>71</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
         <v>201712040324</v>
       </c>
-      <c r="B8" s="2">
-        <v>25</v>
-      </c>
-      <c r="C8" s="2">
+      <c r="B8" s="12">
+        <v>25</v>
+      </c>
+      <c r="C8" s="12">
         <v>19.5</v>
       </c>
-      <c r="D8" s="17">
-        <v>25</v>
-      </c>
-      <c r="E8" s="2">
+      <c r="D8" s="12">
+        <v>25</v>
+      </c>
+      <c r="E8" s="12">
         <v>0</v>
       </c>
-      <c r="F8" s="19"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="3"/>
-    </row>
-    <row r="9" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="F8" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="G8" s="12">
+        <v>15</v>
+      </c>
+      <c r="H8" s="12">
+        <v>87</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
         <v>201712040251</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="12">
         <v>20</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="12">
         <v>16</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="12">
         <v>30</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="12">
         <v>1.5</v>
       </c>
-      <c r="F9" s="19"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="F9" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="G9" s="12">
+        <v>15</v>
+      </c>
+      <c r="H9" s="12">
+        <v>85</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
         <v>201612040420</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="12">
         <v>10</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="12">
         <v>19.5</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="12">
         <v>30</v>
       </c>
-      <c r="E10" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="F10" s="19"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="E10" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="F10" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="G10" s="12">
+        <v>15</v>
+      </c>
+      <c r="H10" s="12">
+        <v>80</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
         <v>201712040022</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="12">
         <v>20</v>
       </c>
-      <c r="C11" s="2">
-        <v>25</v>
-      </c>
-      <c r="D11" s="17">
+      <c r="C11" s="12">
+        <v>25</v>
+      </c>
+      <c r="D11" s="12">
         <v>30</v>
       </c>
-      <c r="E11" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="F11" s="19"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="3"/>
-    </row>
-    <row r="12" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+      <c r="E11" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="F11" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="G11" s="12">
+        <v>15</v>
+      </c>
+      <c r="H11" s="12">
+        <v>95</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="11">
         <v>201522040080</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="12">
         <v>24</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="12">
         <v>18.5</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="12">
         <v>20</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="12">
         <v>0</v>
       </c>
-      <c r="F12" s="19"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="3"/>
-    </row>
-    <row r="13" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="F12" s="12">
+        <v>0</v>
+      </c>
+      <c r="G12" s="12">
+        <v>15</v>
+      </c>
+      <c r="H12" s="12">
+        <v>78</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="11">
         <v>201712040189</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="12">
         <v>20</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="12">
         <v>21</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="12">
         <v>30</v>
       </c>
-      <c r="E13" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="F13" s="19"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="3"/>
-    </row>
-    <row r="14" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="E13" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="F13" s="12">
+        <v>0</v>
+      </c>
+      <c r="G13" s="12">
+        <v>15</v>
+      </c>
+      <c r="H13" s="12">
+        <v>89</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="11">
         <v>201622040023</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="12">
         <v>24</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="12">
         <v>22.5</v>
       </c>
-      <c r="D14" s="17">
-        <v>25</v>
-      </c>
-      <c r="E14" s="2">
+      <c r="D14" s="12">
+        <v>25</v>
+      </c>
+      <c r="E14" s="12">
         <v>1</v>
       </c>
-      <c r="F14" s="19"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="3"/>
-    </row>
-    <row r="15" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+      <c r="F14" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="G14" s="12">
+        <v>15</v>
+      </c>
+      <c r="H14" s="12">
+        <v>90</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="11">
         <v>201712040421</v>
       </c>
-      <c r="B15" s="2">
-        <v>15</v>
-      </c>
-      <c r="C15" s="2">
-        <v>25</v>
-      </c>
-      <c r="D15" s="17">
-        <v>25</v>
-      </c>
-      <c r="E15" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="F15" s="19"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="3"/>
-    </row>
-    <row r="16" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+      <c r="B15" s="12">
+        <v>15</v>
+      </c>
+      <c r="C15" s="12">
+        <v>25</v>
+      </c>
+      <c r="D15" s="12">
+        <v>25</v>
+      </c>
+      <c r="E15" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="F15" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="G15" s="12">
+        <v>15</v>
+      </c>
+      <c r="H15" s="12">
+        <v>85</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="11">
         <v>201412040264</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="12">
         <v>13</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="12">
         <v>20</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="12">
         <v>30</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="12">
         <v>1</v>
       </c>
-      <c r="F16" s="19"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="3"/>
-    </row>
-    <row r="17" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+      <c r="F16" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="G16" s="12">
+        <v>15</v>
+      </c>
+      <c r="H16" s="12">
+        <v>81</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="11">
         <v>201712040170</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="12">
         <v>20</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="12">
         <v>15.5</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="12">
         <v>30</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="12">
         <v>1</v>
       </c>
-      <c r="F17" s="19"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="3"/>
-    </row>
-    <row r="18" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+      <c r="F17" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="G17" s="12">
+        <v>15</v>
+      </c>
+      <c r="H17" s="12">
+        <v>84</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="11">
         <v>201712040227</v>
       </c>
-      <c r="B18" s="2">
-        <v>15</v>
-      </c>
-      <c r="C18" s="2">
+      <c r="B18" s="12">
+        <v>15</v>
+      </c>
+      <c r="C18" s="12">
         <v>17</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D18" s="12">
         <v>30</v>
       </c>
-      <c r="E18" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="F18" s="19"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="3"/>
-    </row>
-    <row r="19" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+      <c r="E18" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="F18" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="G18" s="12">
+        <v>15</v>
+      </c>
+      <c r="H18" s="12">
+        <v>82</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="11">
         <v>201717060358</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="12">
         <v>22</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="12">
         <v>21</v>
       </c>
-      <c r="D19" s="18">
-        <v>25</v>
-      </c>
-      <c r="E19" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="F19" s="19"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="3"/>
-    </row>
-    <row r="20" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+      <c r="D19" s="12">
+        <v>25</v>
+      </c>
+      <c r="E19" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="F19" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="G19" s="12">
+        <v>15</v>
+      </c>
+      <c r="H19" s="12">
+        <v>88</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="11">
         <v>201522040463</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="12">
         <v>20</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="12">
         <v>19.5</v>
       </c>
-      <c r="D20" s="18">
+      <c r="D20" s="12">
         <v>30</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="12">
         <v>1.5</v>
       </c>
-      <c r="F20" s="19"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="3"/>
-    </row>
-    <row r="21" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+      <c r="F20" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="G20" s="12">
+        <v>15</v>
+      </c>
+      <c r="H20" s="12">
+        <v>89</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="11">
         <v>20183008679</v>
       </c>
-      <c r="B21" s="2">
-        <v>25</v>
-      </c>
-      <c r="C21" s="2">
+      <c r="B21" s="12">
+        <v>25</v>
+      </c>
+      <c r="C21" s="12">
         <v>13</v>
       </c>
-      <c r="D21" s="18">
-        <v>25</v>
-      </c>
-      <c r="E21" s="2">
+      <c r="D21" s="12">
+        <v>25</v>
+      </c>
+      <c r="E21" s="12">
         <v>0</v>
       </c>
-      <c r="F21" s="19"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="3"/>
-    </row>
-    <row r="22" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+      <c r="F21" s="12">
+        <v>0</v>
+      </c>
+      <c r="G21" s="12">
+        <v>15</v>
+      </c>
+      <c r="H21" s="12">
+        <v>78</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="11">
         <v>201622040112</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="12">
         <v>18</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="12">
         <v>18.5</v>
       </c>
-      <c r="D22" s="18">
+      <c r="D22" s="12">
         <v>30</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="12">
         <v>1</v>
       </c>
-      <c r="F22" s="19"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="3"/>
-    </row>
-    <row r="23" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+      <c r="F22" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="G22" s="12">
+        <v>15</v>
+      </c>
+      <c r="H22" s="12">
+        <v>84</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="11">
         <v>201712040456</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="12">
         <v>20</v>
       </c>
-      <c r="C23" s="2">
-        <v>25</v>
-      </c>
-      <c r="D23" s="18">
+      <c r="C23" s="12">
+        <v>25</v>
+      </c>
+      <c r="D23" s="12">
         <v>30</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="12">
         <v>1.5</v>
       </c>
-      <c r="F23" s="19"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="3"/>
-    </row>
-    <row r="24" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+      <c r="F23" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="G23" s="12">
+        <v>15</v>
+      </c>
+      <c r="H23" s="12">
+        <v>94</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="11">
         <v>201712040014</v>
       </c>
-      <c r="B24" s="2">
-        <v>25</v>
-      </c>
-      <c r="C24" s="2">
-        <v>25</v>
-      </c>
-      <c r="D24" s="18">
-        <v>25</v>
-      </c>
-      <c r="E24" s="2">
+      <c r="B24" s="12">
+        <v>25</v>
+      </c>
+      <c r="C24" s="12">
+        <v>25</v>
+      </c>
+      <c r="D24" s="12">
+        <v>25</v>
+      </c>
+      <c r="E24" s="12">
         <v>1.5</v>
       </c>
-      <c r="F24" s="19"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="3"/>
-    </row>
-    <row r="25" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+      <c r="F24" s="12">
+        <v>0</v>
+      </c>
+      <c r="G24" s="12">
+        <v>15</v>
+      </c>
+      <c r="H24" s="12">
+        <v>92</v>
+      </c>
+      <c r="I24" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="11">
         <v>201712040472</v>
       </c>
-      <c r="B25" s="2">
-        <v>25</v>
-      </c>
-      <c r="C25" s="2">
+      <c r="B25" s="12">
+        <v>25</v>
+      </c>
+      <c r="C25" s="12">
         <v>17</v>
       </c>
-      <c r="D25" s="18">
-        <v>25</v>
-      </c>
-      <c r="E25" s="2">
+      <c r="D25" s="12">
+        <v>25</v>
+      </c>
+      <c r="E25" s="12">
         <v>1</v>
       </c>
-      <c r="F25" s="19"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="3"/>
-    </row>
-    <row r="26" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+      <c r="F25" s="12">
+        <v>0</v>
+      </c>
+      <c r="G25" s="12">
+        <v>15</v>
+      </c>
+      <c r="H25" s="12">
+        <v>83</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="11">
         <v>201622040120</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="12">
         <v>20</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="12">
         <v>18.5</v>
       </c>
-      <c r="D26" s="18">
+      <c r="D26" s="12">
         <v>30</v>
       </c>
-      <c r="E26" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="F26" s="19"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="3"/>
-    </row>
-    <row r="27" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+      <c r="E26" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="F26" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="G26" s="12">
+        <v>15</v>
+      </c>
+      <c r="H26" s="12">
+        <v>88</v>
+      </c>
+      <c r="I26" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="11">
         <v>201712040286</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="12">
         <v>24</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="12">
         <v>21</v>
       </c>
-      <c r="D27" s="18">
-        <v>25</v>
-      </c>
-      <c r="E27" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="F27" s="19"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="3"/>
-    </row>
-    <row r="28" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+      <c r="D27" s="12">
+        <v>25</v>
+      </c>
+      <c r="E27" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="F27" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="G27" s="12">
+        <v>15</v>
+      </c>
+      <c r="H27" s="12">
+        <v>90</v>
+      </c>
+      <c r="I27" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="11">
         <v>201522040170</v>
       </c>
-      <c r="B28" s="2">
-        <v>15</v>
-      </c>
-      <c r="C28" s="2">
-        <v>25</v>
-      </c>
-      <c r="D28" s="18">
+      <c r="B28" s="12">
+        <v>15</v>
+      </c>
+      <c r="C28" s="12">
+        <v>25</v>
+      </c>
+      <c r="D28" s="12">
         <v>30</v>
       </c>
-      <c r="E28" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="F28" s="19"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="3"/>
-    </row>
-    <row r="29" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+      <c r="E28" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="F28" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="G28" s="12">
+        <v>15</v>
+      </c>
+      <c r="H28" s="12">
+        <v>90</v>
+      </c>
+      <c r="I28" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="11">
         <v>201712040278</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="12">
         <v>20</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="12">
         <v>21</v>
       </c>
-      <c r="D29" s="18">
+      <c r="D29" s="12">
         <v>30</v>
       </c>
-      <c r="E29" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="F29" s="19"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="3"/>
-    </row>
-    <row r="30" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+      <c r="E29" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="F29" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="G29" s="12">
+        <v>15</v>
+      </c>
+      <c r="H29" s="12">
+        <v>91</v>
+      </c>
+      <c r="I29" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="11">
         <v>201622040295</v>
       </c>
-      <c r="B30" s="2">
-        <v>25</v>
-      </c>
-      <c r="C30" s="2">
+      <c r="B30" s="12">
+        <v>25</v>
+      </c>
+      <c r="C30" s="12">
         <v>22.5</v>
       </c>
-      <c r="D30" s="18">
+      <c r="D30" s="12">
         <v>30</v>
       </c>
-      <c r="E30" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="F30" s="19"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="3"/>
-    </row>
-    <row r="32" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="G32" s="14" t="s">
+      <c r="E30" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="F30" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="G30" s="12">
+        <v>15</v>
+      </c>
+      <c r="H30" s="12">
+        <v>98</v>
+      </c>
+      <c r="I30" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H32" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="H32" s="15"/>
-    </row>
-    <row r="33" spans="7:8" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="G33" s="16" t="s">
+      <c r="I32" s="16"/>
+      <c r="J32" s="14"/>
+    </row>
+    <row r="33" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H33" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H33" s="15"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="14"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -1292,92 +1562,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
     </row>
     <row r="4" spans="2:6" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
     </row>
     <row r="6" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10" t="s">
+      <c r="C6" s="1"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
     </row>
     <row r="8" spans="2:6" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12">
+      <c r="C8" s="4"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7">
         <v>1</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>